<commit_message>
updated grade for project2
</commit_message>
<xml_diff>
--- a/project2-grading.xlsx
+++ b/project2-grading.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Area</t>
   </si>
@@ -89,6 +89,18 @@
   </si>
   <si>
     <t>The functions within the program should be much better organized. Functions are too long, with many places not properly indented. It is very hard to read the code.</t>
+  </si>
+  <si>
+    <t>Updated comments</t>
+  </si>
+  <si>
+    <t>Thank you for taking time to talk to me. The discussion cleared a lot of confusion. Timer implementation is still off a bit.</t>
+  </si>
+  <si>
+    <t>Very good! Again, the CRC mechanism is hidden in the crowded code, it is hard to find!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timer implementation is incorrect in logic, though your program mimics certain behavior of the timer. </t>
   </si>
 </sst>
 </file>
@@ -469,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -578,6 +590,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -951,10 +969,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -963,37 +981,38 @@
     <col min="3" max="3" width="10.75" customWidth="1"/>
     <col min="4" max="4" width="9.125" customWidth="1"/>
     <col min="5" max="5" width="21.625" customWidth="1"/>
+    <col min="6" max="6" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="39" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1006,8 +1025,11 @@
       <c r="E5" s="17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="41"/>
       <c r="B6" s="3" t="s">
         <v>4</v>
@@ -1016,7 +1038,7 @@
       <c r="D6" s="15"/>
       <c r="E6" s="18"/>
     </row>
-    <row r="7" spans="1:5" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A7" s="41"/>
       <c r="B7" s="22" t="s">
         <v>15</v>
@@ -1024,21 +1046,25 @@
       <c r="C7" s="9">
         <v>25</v>
       </c>
-      <c r="D7" s="6">
-        <v>22</v>
+      <c r="D7" s="44">
+        <v>24</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="43" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="41"/>
       <c r="B8" s="4"/>
       <c r="C8" s="11"/>
       <c r="D8" s="8"/>
       <c r="E8" s="18"/>
-    </row>
-    <row r="9" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="41"/>
       <c r="B9" s="22" t="s">
         <v>12</v>
@@ -1052,15 +1078,17 @@
       <c r="E9" s="18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="41"/>
       <c r="B10" s="35"/>
       <c r="C10" s="10"/>
       <c r="D10" s="7"/>
       <c r="E10" s="18"/>
-    </row>
-    <row r="11" spans="1:5" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A11" s="41"/>
       <c r="B11" s="23" t="s">
         <v>13</v>
@@ -1069,20 +1097,24 @@
         <v>15</v>
       </c>
       <c r="D11" s="7">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="41"/>
       <c r="B12" s="4"/>
       <c r="C12" s="11"/>
       <c r="D12" s="7"/>
       <c r="E12" s="18"/>
-    </row>
-    <row r="13" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="41"/>
       <c r="B13" s="40" t="s">
         <v>14</v>
@@ -1091,20 +1123,24 @@
         <v>10</v>
       </c>
       <c r="D13" s="6">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
       <c r="B14" s="40"/>
       <c r="C14" s="10"/>
       <c r="D14" s="19"/>
       <c r="E14" s="18"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="41"/>
       <c r="B15" s="3" t="s">
         <v>9</v>
@@ -1112,8 +1148,9 @@
       <c r="C15" s="14"/>
       <c r="D15" s="15"/>
       <c r="E15" s="18"/>
-    </row>
-    <row r="16" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="41"/>
       <c r="B16" s="22" t="s">
         <v>6</v>
@@ -1127,15 +1164,17 @@
       <c r="E16" s="18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="41"/>
       <c r="B17" s="36"/>
       <c r="C17" s="37"/>
       <c r="D17" s="38"/>
       <c r="E17" s="18"/>
-    </row>
-    <row r="18" spans="1:5" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="41"/>
       <c r="B18" s="23" t="s">
         <v>7</v>
@@ -1149,15 +1188,17 @@
       <c r="E18" s="18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27"/>
       <c r="B19" s="29"/>
       <c r="C19" s="31"/>
       <c r="D19" s="30"/>
       <c r="E19" s="18"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="32" t="s">
         <v>8</v>
@@ -1166,18 +1207,20 @@
         <v>10</v>
       </c>
       <c r="D20" s="28">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E20" s="18"/>
-    </row>
-    <row r="21" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27"/>
       <c r="B21" s="23"/>
       <c r="C21" s="34"/>
       <c r="D21" s="28"/>
       <c r="E21" s="18"/>
-    </row>
-    <row r="22" spans="1:5" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="21" t="s">
         <v>5</v>
       </c>
@@ -1187,21 +1230,22 @@
       </c>
       <c r="D22" s="26">
         <f>SUM(D7:D21)</f>
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="E22" s="18"/>
-    </row>
-    <row r="23" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="42"/>
       <c r="B23" s="24"/>
       <c r="E23" s="18"/>
     </row>
-    <row r="24" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="42"/>
       <c r="B24" s="20"/>
       <c r="E24" s="18"/>
     </row>
-    <row r="25" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="42"/>
     </row>
   </sheetData>

</xml_diff>